<commit_message>
Updates for camera ready
</commit_message>
<xml_diff>
--- a/results/experiments.xlsx
+++ b/results/experiments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jonkopinguniversity.sharepoint.com/sites/G-Arbetsplanering/Delade dokument/Egna Artiklar/LIME-artikel (AMAI)/amai-calibrating-explanations-2023/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="916" documentId="13_ncr:40009_{88C8AC52-A149-4AF4-B2D1-722DED437099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9104444-FAE6-49F4-BCE1-0FF5CDCC7833}"/>
+  <xr:revisionPtr revIDLastSave="953" documentId="13_ncr:40009_{88C8AC52-A149-4AF4-B2D1-722DED437099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB0BE2C1-36F2-4D93-86A0-C0F2F34ECFD7}"/>
   <bookViews>
-    <workbookView xWindow="-5010" yWindow="-16320" windowWidth="38640" windowHeight="15990" tabRatio="784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All tables colored for Findings" sheetId="5" r:id="rId1"/>
@@ -33,12 +33,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="49">
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>Table 3</t>
+  </si>
+  <si>
+    <t>Table 4 ECE LIME</t>
+  </si>
+  <si>
+    <t>Table 5 Log loss LIME</t>
+  </si>
+  <si>
+    <t>#instances</t>
+  </si>
+  <si>
+    <t>#features</t>
+  </si>
+  <si>
+    <t>inst/feat</t>
+  </si>
+  <si>
+    <t>maj/min</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>Expected Calibration Error</t>
+  </si>
+  <si>
+    <t>Log loss</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
   <si>
     <t>RF</t>
   </si>
   <si>
     <t>xGB</t>
+  </si>
+  <si>
+    <t>Datasets</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>VA</t>
   </si>
   <si>
     <t>colic</t>
@@ -77,10 +134,16 @@
     <t>je4243</t>
   </si>
   <si>
+    <t>kc1</t>
+  </si>
+  <si>
     <t>kc2</t>
   </si>
   <si>
     <t>kc3</t>
+  </si>
+  <si>
+    <t>liver</t>
   </si>
   <si>
     <t>pc1req</t>
@@ -113,67 +176,10 @@
     <t>Mean</t>
   </si>
   <si>
-    <t>Datasets</t>
+    <t>-</t>
   </si>
   <si>
-    <t>Top</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>UC</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>VA</t>
-  </si>
-  <si>
-    <t>kc1</t>
-  </si>
-  <si>
-    <t>liver</t>
-  </si>
-  <si>
-    <t>Expected Calibration Error</t>
-  </si>
-  <si>
-    <t>AUC</t>
-  </si>
-  <si>
-    <t>#instances</t>
-  </si>
-  <si>
-    <t>#features</t>
-  </si>
-  <si>
-    <t>inst/feat</t>
-  </si>
-  <si>
-    <t>maj/min</t>
-  </si>
-  <si>
-    <t>Table 1</t>
-  </si>
-  <si>
-    <t>Table 2</t>
-  </si>
-  <si>
-    <t>Table 3</t>
-  </si>
-  <si>
-    <t>ACC</t>
-  </si>
-  <si>
-    <t>Table 4 ECE LIME</t>
-  </si>
-  <si>
-    <t>Table 5 Log loss LIME</t>
-  </si>
-  <si>
-    <t>Log loss</t>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -181,10 +187,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode=".000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode=".000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +321,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -780,13 +794,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -795,54 +809,46 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -857,6 +863,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1215,426 +1225,419 @@
   <dimension ref="A1:BL56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="AE26" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AV30" sqref="AV30:AY30"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="X2" sqref="X2:AC2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="5.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="23" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="4.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="30" max="35" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="4.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="4.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="42" max="47" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="48" max="50" width="4.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="5.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="52" max="53" width="4.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="9.140625" style="9"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" customWidth="1"/>
+    <col min="9" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="35" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="38" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="42" max="47" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="50" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="29"/>
-      <c r="AP1" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="AQ1" s="28"/>
-      <c r="AR1" s="28"/>
-      <c r="AS1" s="28"/>
-      <c r="AT1" s="28"/>
-      <c r="AU1" s="28"/>
-      <c r="AV1" s="28"/>
-      <c r="AW1" s="28"/>
-      <c r="AX1" s="28"/>
-      <c r="AY1" s="28"/>
-      <c r="AZ1" s="28"/>
-      <c r="BA1" s="29"/>
-      <c r="BB1" s="9"/>
-      <c r="BC1" s="9"/>
-      <c r="BD1" s="9"/>
-      <c r="BE1" s="9"/>
-      <c r="BF1" s="9"/>
-      <c r="BG1" s="9"/>
-      <c r="BH1" s="9"/>
-      <c r="BI1" s="9"/>
-      <c r="BJ1" s="9"/>
-      <c r="BK1" s="9"/>
-      <c r="BL1" s="9"/>
+    <row r="1" spans="1:64" ht="14.45" customHeight="1" thickBot="1">
+      <c r="B1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE1" s="22"/>
+      <c r="AF1" s="22"/>
+      <c r="AG1" s="22"/>
+      <c r="AH1" s="22"/>
+      <c r="AI1" s="22"/>
+      <c r="AJ1" s="22"/>
+      <c r="AK1" s="22"/>
+      <c r="AL1" s="22"/>
+      <c r="AM1" s="22"/>
+      <c r="AN1" s="22"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ1" s="22"/>
+      <c r="AR1" s="22"/>
+      <c r="AS1" s="22"/>
+      <c r="AT1" s="22"/>
+      <c r="AU1" s="22"/>
+      <c r="AV1" s="22"/>
+      <c r="AW1" s="22"/>
+      <c r="AX1" s="22"/>
+      <c r="AY1" s="22"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="24"/>
     </row>
-    <row r="2" spans="1:64" customFormat="1" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="22.15" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25"/>
-      <c r="AG2" s="25"/>
-      <c r="AH2" s="25"/>
-      <c r="AI2" s="26"/>
-      <c r="AJ2" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="26"/>
-      <c r="AP2" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="AQ2" s="25"/>
-      <c r="AR2" s="25"/>
-      <c r="AS2" s="25"/>
-      <c r="AT2" s="25"/>
-      <c r="AU2" s="26"/>
-      <c r="AV2" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="AW2" s="25"/>
-      <c r="AX2" s="25"/>
-      <c r="AY2" s="25"/>
-      <c r="AZ2" s="25"/>
-      <c r="BA2" s="26"/>
+      <c r="B2" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19"/>
+      <c r="AG2" s="19"/>
+      <c r="AH2" s="19"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="19"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ2" s="19"/>
+      <c r="AR2" s="19"/>
+      <c r="AS2" s="19"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="19"/>
+      <c r="AY2" s="19"/>
+      <c r="AZ2" s="19"/>
+      <c r="BA2" s="20"/>
     </row>
-    <row r="3" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64">
       <c r="A3" s="1"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="V3" s="25"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="26"/>
-      <c r="AD3" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="26"/>
-      <c r="AJ3" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="26"/>
-      <c r="AP3" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="25"/>
-      <c r="AR3" s="25"/>
-      <c r="AS3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT3" s="25"/>
-      <c r="AU3" s="26"/>
-      <c r="AV3" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="25"/>
-      <c r="AX3" s="25"/>
-      <c r="AY3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ3" s="25"/>
-      <c r="BA3" s="26"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="19"/>
+      <c r="W3" s="20"/>
+      <c r="X3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="20"/>
+      <c r="AD3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH3" s="19"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK3" s="19"/>
+      <c r="AL3" s="19"/>
+      <c r="AM3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AN3" s="19"/>
+      <c r="AO3" s="20"/>
+      <c r="AP3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ3" s="19"/>
+      <c r="AR3" s="19"/>
+      <c r="AS3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT3" s="19"/>
+      <c r="AU3" s="20"/>
+      <c r="AV3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW3" s="19"/>
+      <c r="AX3" s="19"/>
+      <c r="AY3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ3" s="19"/>
+      <c r="BA3" s="20"/>
     </row>
-    <row r="4" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" s="3" customFormat="1">
       <c r="A4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="34"/>
+        <v>17</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AA4" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="AB4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="AC4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AD4" s="7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="AE4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="AF4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AG4" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="AH4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="AI4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AJ4" s="7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="AK4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="AL4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AM4" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="AN4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="AO4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AP4" s="7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="AQ4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="AR4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AS4" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="AT4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="AU4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AV4" s="7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="AW4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="AX4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="AY4" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="AZ4" s="6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="BA4" s="6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="BB4"/>
       <c r="BC4"/>
@@ -1648,9 +1651,9 @@
       <c r="BK4"/>
       <c r="BL4"/>
     </row>
-    <row r="5" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>375</v>
@@ -1658,47 +1661,47 @@
       <c r="C5">
         <v>59</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="12">
         <f>B5/C5</f>
         <v>6.3559322033898304</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>1.664179104477612</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>0.83697478991596597</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="10">
         <v>0.82605042016806696</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="10">
         <v>0.82408963585434103</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <v>0.84033613445378097</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="10">
         <v>0.83193277310924296</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="10">
         <v>0.82352941176470495</v>
       </c>
-      <c r="L5" s="12">
+      <c r="L5" s="11">
         <v>0.75357040993297297</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="10">
         <v>0.75506367233850402</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="10">
         <v>0.748534836997233</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="10">
         <v>0.75485380116959</v>
       </c>
-      <c r="P5" s="11">
+      <c r="P5" s="10">
         <v>0.72452300785634105</v>
       </c>
-      <c r="Q5" s="11">
+      <c r="Q5" s="10">
         <v>0.75010797969981602</v>
       </c>
       <c r="R5" s="8">
@@ -1719,7 +1722,7 @@
       <c r="W5" s="5">
         <v>3.6294955061096403E-2</v>
       </c>
-      <c r="X5" s="10">
+      <c r="X5" s="9">
         <v>0.40214283267553602</v>
       </c>
       <c r="Y5" s="4">
@@ -1810,9 +1813,9 @@
         <v>0.401130730319605</v>
       </c>
     </row>
-    <row r="6" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>690</v>
@@ -1820,47 +1823,47 @@
       <c r="C6">
         <v>42</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <f t="shared" ref="D6:D29" si="0">B6/C6</f>
         <v>16.428571428571427</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="12">
         <v>1.2475570032573291</v>
       </c>
       <c r="F6" s="8">
         <v>0.84956521739130397</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="5">
         <v>0.84710144927536202</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="5">
         <v>0.83362318840579697</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="5">
         <v>0.84492753623188399</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="5">
         <v>0.85362318840579698</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="5">
         <v>0.83188405797101395</v>
       </c>
       <c r="L6" s="8">
         <v>0.77211945721405995</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="5">
         <v>0.73133078460546697</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="5">
         <v>0.76938441045199202</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="5">
         <v>0.76614674339943201</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="5">
         <v>0.53956193582006695</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="5">
         <v>0.73123423044575198</v>
       </c>
       <c r="R6" s="8">
@@ -1881,7 +1884,7 @@
       <c r="W6" s="5">
         <v>6.1222804845243201E-2</v>
       </c>
-      <c r="X6" s="10">
+      <c r="X6" s="9">
         <v>0.41577081067590699</v>
       </c>
       <c r="Y6" s="4">
@@ -1972,9 +1975,9 @@
         <v>0.40165195411744398</v>
       </c>
     </row>
-    <row r="7" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>768</v>
@@ -1982,47 +1985,47 @@
       <c r="C7">
         <v>8</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="12">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="12">
         <v>1.8656716417910448</v>
       </c>
       <c r="F7" s="8">
         <v>0.75924479166666603</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="5">
         <v>0.75416666666666599</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="5">
         <v>0.75755208333333302</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="5">
         <v>0.73567708333333304</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="5">
         <v>0.73567708333333304</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="5">
         <v>0.71484375</v>
       </c>
       <c r="L7" s="8">
         <v>0.72832023947645896</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="5">
         <v>0.72832258038556896</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="5">
         <v>0.70716269446390101</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="5">
         <v>0.71366668119795895</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P7" s="5">
         <v>0.67339465539038301</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q7" s="5">
         <v>0.72970781246101202</v>
       </c>
       <c r="R7" s="8">
@@ -2043,7 +2046,7 @@
       <c r="W7" s="5">
         <v>4.59703796053266E-2</v>
       </c>
-      <c r="X7" s="10">
+      <c r="X7" s="9">
         <v>0.49340894318427903</v>
       </c>
       <c r="Y7" s="4">
@@ -2134,9 +2137,9 @@
         <v>0.508672054656783</v>
       </c>
     </row>
-    <row r="8" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>955</v>
@@ -2144,47 +2147,47 @@
       <c r="C8">
         <v>27</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="12">
         <f t="shared" si="0"/>
         <v>35.370370370370374</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="12">
         <v>2.3745583038869258</v>
       </c>
       <c r="F8" s="8">
         <v>0.66712041884816697</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="5">
         <v>0.701884816753926</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="5">
         <v>0.69979057591622995</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="5">
         <v>0.62303664921465896</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="5">
         <v>0.70366492146596804</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="5">
         <v>0.70261780104712002</v>
       </c>
       <c r="L8" s="8">
         <v>0.640672836854279</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="5">
         <v>0.61365549850260204</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="5">
         <v>0.61793601316815605</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="5">
         <v>0.63469654528478003</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="5">
         <v>0.55029025744573401</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="5">
         <v>0.57364717365294604</v>
       </c>
       <c r="R8" s="8">
@@ -2205,7 +2208,7 @@
       <c r="W8" s="5">
         <v>9.2259226981258394E-3</v>
       </c>
-      <c r="X8" s="10">
+      <c r="X8" s="9">
         <v>0.65702791389032</v>
       </c>
       <c r="Y8" s="4">
@@ -2296,9 +2299,9 @@
         <v>0.60130184301519796</v>
       </c>
     </row>
-    <row r="9" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>283</v>
@@ -2306,47 +2309,47 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="12">
         <f t="shared" si="0"/>
         <v>94.333333333333329</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="12">
         <v>2.5822784810126582</v>
       </c>
       <c r="F9" s="8">
         <v>0.66961130742049402</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="5">
         <v>0.719434628975265</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="5">
         <v>0.71837455830388697</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="5">
         <v>0.58657243816254401</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="5">
         <v>0.72084805653710204</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="5">
         <v>0.72084805653710204</v>
       </c>
       <c r="L9" s="8">
         <v>0.64156279542279804</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="5">
         <v>0.62448502521366001</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="5">
         <v>0.64566707050109795</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="5">
         <v>0.59939759036144502</v>
       </c>
-      <c r="P9" s="13">
+      <c r="P9" s="5">
         <v>0.45730950608091298</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="Q9" s="5">
         <v>0.54172871680317702</v>
       </c>
       <c r="R9" s="8">
@@ -2367,7 +2370,7 @@
       <c r="W9" s="5">
         <v>7.7190531016238503E-2</v>
       </c>
-      <c r="X9" s="10">
+      <c r="X9" s="9">
         <v>0.70974276468487696</v>
       </c>
       <c r="Y9" s="4">
@@ -2458,9 +2461,9 @@
         <v>0.59372133448720699</v>
       </c>
     </row>
-    <row r="10" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>302</v>
@@ -2468,47 +2471,47 @@
       <c r="C10">
         <v>22</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="12">
         <f t="shared" si="0"/>
         <v>13.727272727272727</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="12">
         <v>1.1884057971014492</v>
       </c>
       <c r="F10" s="8">
         <v>0.82649006622516497</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="5">
         <v>0.82218543046357595</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="5">
         <v>0.81125827814569496</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="5">
         <v>0.78807947019867497</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="5">
         <v>0.77814569536423805</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="5">
         <v>0.77152317880794696</v>
       </c>
       <c r="L10" s="8">
         <v>0.77284877177529798</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="5">
         <v>0.74961469838477002</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="5">
         <v>0.74690941639813802</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="5">
         <v>0.78472951680672198</v>
       </c>
-      <c r="P10" s="13">
+      <c r="P10" s="5">
         <v>0.70511273420133302</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q10" s="5">
         <v>0.74339117994650705</v>
       </c>
       <c r="R10" s="8">
@@ -2529,7 +2532,7 @@
       <c r="W10" s="5">
         <v>3.7539422684750003E-2</v>
       </c>
-      <c r="X10" s="10">
+      <c r="X10" s="9">
         <v>0.39576211718815701</v>
       </c>
       <c r="Y10" s="4">
@@ -2620,9 +2623,9 @@
         <v>0.45331906541722999</v>
       </c>
     </row>
-    <row r="11" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>293</v>
@@ -2630,47 +2633,47 @@
       <c r="C11">
         <v>20</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="12">
         <f t="shared" si="0"/>
         <v>14.65</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="12">
         <v>1.7641509433962264</v>
       </c>
       <c r="F11" s="8">
         <v>0.78907849829351495</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="5">
         <v>0.81092150170648403</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="5">
         <v>0.78839590443686003</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="5">
         <v>0.720136518771331</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="5">
         <v>0.77133105802047697</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="5">
         <v>0.76791808873720102</v>
       </c>
       <c r="L11" s="8">
         <v>0.76552754168486303</v>
       </c>
-      <c r="M11" s="13">
+      <c r="M11" s="5">
         <v>0.71581108923166603</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="5">
         <v>0.73887131685518703</v>
       </c>
-      <c r="O11" s="13">
+      <c r="O11" s="5">
         <v>0.74586752976534498</v>
       </c>
-      <c r="P11" s="13">
+      <c r="P11" s="5">
         <v>0.63003566239598396</v>
       </c>
-      <c r="Q11" s="13">
+      <c r="Q11" s="5">
         <v>0.65098039215686199</v>
       </c>
       <c r="R11" s="8">
@@ -2691,7 +2694,7 @@
       <c r="W11" s="5">
         <v>7.4301750205279196E-2</v>
       </c>
-      <c r="X11" s="10">
+      <c r="X11" s="9">
         <v>0.46643688202891298</v>
       </c>
       <c r="Y11" s="4">
@@ -2782,9 +2785,9 @@
         <v>0.51452084158843003</v>
       </c>
     </row>
-    <row r="12" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>270</v>
@@ -2792,47 +2795,47 @@
       <c r="C12">
         <v>13</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <f t="shared" si="0"/>
         <v>20.76923076923077</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="12">
         <v>1.25</v>
       </c>
       <c r="F12" s="8">
         <v>0.82962962962962905</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="5">
         <v>0.81851851851851798</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="5">
         <v>0.81</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="5">
         <v>0.80740740740740702</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="5">
         <v>0.80370370370370303</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="5">
         <v>0.79259259259259196</v>
       </c>
       <c r="L12" s="8">
         <v>0.75860636645962698</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="5">
         <v>0.71613953273617104</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="5">
         <v>0.70554606299317801</v>
       </c>
-      <c r="O12" s="13">
+      <c r="O12" s="5">
         <v>0.77425899788285102</v>
       </c>
-      <c r="P12" s="13">
+      <c r="P12" s="5">
         <v>0.64707416746369795</v>
       </c>
-      <c r="Q12" s="13">
+      <c r="Q12" s="5">
         <v>0.705065086782376</v>
       </c>
       <c r="R12" s="8">
@@ -2853,7 +2856,7 @@
       <c r="W12" s="5">
         <v>7.5767063121828696E-2</v>
       </c>
-      <c r="X12" s="10">
+      <c r="X12" s="9">
         <v>0.416843801624461</v>
       </c>
       <c r="Y12" s="4">
@@ -2944,9 +2947,9 @@
         <v>0.45235330491784398</v>
       </c>
     </row>
-    <row r="13" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <v>155</v>
@@ -2954,47 +2957,47 @@
       <c r="C13">
         <v>19</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="12">
         <f t="shared" si="0"/>
         <v>8.1578947368421044</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="12">
         <v>3.84375</v>
       </c>
       <c r="F13" s="8">
         <v>0.83419354838709603</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="5">
         <v>0.825806451612903</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="5">
         <v>0.82451612903225802</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="5">
         <v>0.8</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="5">
         <v>0.81290322580645102</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="5">
         <v>0.76774193548387004</v>
       </c>
       <c r="L13" s="8">
         <v>0.82634870192987597</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13" s="5">
         <v>0.79741608796296204</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="5">
         <v>0.81101128831814395</v>
       </c>
-      <c r="O13" s="13">
+      <c r="O13" s="5">
         <v>0.79916753381893801</v>
       </c>
-      <c r="P13" s="13">
+      <c r="P13" s="5">
         <v>0.73453749315818295</v>
       </c>
-      <c r="Q13" s="13">
+      <c r="Q13" s="5">
         <v>0.80380485527544299</v>
       </c>
       <c r="R13" s="8">
@@ -3015,7 +3018,7 @@
       <c r="W13" s="5">
         <v>0.119312449472565</v>
       </c>
-      <c r="X13" s="10">
+      <c r="X13" s="9">
         <v>0.34680011309179898</v>
       </c>
       <c r="Y13" s="4">
@@ -3106,9 +3109,9 @@
         <v>0.44076239981587401</v>
       </c>
     </row>
-    <row r="14" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>350</v>
@@ -3116,47 +3119,47 @@
       <c r="C14">
         <v>33</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="12">
         <f t="shared" si="0"/>
         <v>10.606060606060606</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="12">
         <v>1.8</v>
       </c>
       <c r="F14" s="8">
         <v>0.93657142857142806</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="5">
         <v>0.93</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="5">
         <v>0.92257142857142804</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="5">
         <v>0.90857142857142803</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="5">
         <v>0.91142857142857103</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="5">
         <v>0.91428571428571404</v>
       </c>
       <c r="L14" s="8">
         <v>0.86319388332811098</v>
       </c>
-      <c r="M14" s="13">
+      <c r="M14" s="5">
         <v>0.83660490924480302</v>
       </c>
-      <c r="N14" s="13">
+      <c r="N14" s="5">
         <v>0.84583782350675796</v>
       </c>
-      <c r="O14" s="13">
+      <c r="O14" s="5">
         <v>0.85151336477987405</v>
       </c>
-      <c r="P14" s="13">
+      <c r="P14" s="5">
         <v>0.68014966123976095</v>
       </c>
-      <c r="Q14" s="13">
+      <c r="Q14" s="5">
         <v>0.74687499999999996</v>
       </c>
       <c r="R14" s="8">
@@ -3177,7 +3180,7 @@
       <c r="W14" s="5">
         <v>7.10352188561644E-2</v>
       </c>
-      <c r="X14" s="10">
+      <c r="X14" s="9">
         <v>0.21682667828236751</v>
       </c>
       <c r="Y14" s="4">
@@ -3268,9 +3271,9 @@
         <v>0.280180448161994</v>
       </c>
     </row>
-    <row r="15" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>270</v>
@@ -3278,47 +3281,47 @@
       <c r="C15">
         <v>8</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="12">
         <f t="shared" si="0"/>
         <v>33.75</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="12">
         <v>1.0149253731343284</v>
       </c>
       <c r="F15" s="8">
         <v>0.75296296296296295</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="5">
         <v>0.73148148148148096</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="5">
         <v>0.72666666666666602</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="5">
         <v>0.70370370370370305</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="5">
         <v>0.74444444444444402</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="5">
         <v>0.75555555555555498</v>
       </c>
       <c r="L15" s="8">
         <v>0.66273282443873904</v>
       </c>
-      <c r="M15" s="13">
+      <c r="M15" s="5">
         <v>0.67961763422086396</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="5">
         <v>0.67027278453212602</v>
       </c>
-      <c r="O15" s="13">
+      <c r="O15" s="5">
         <v>0.68888157894736801</v>
       </c>
-      <c r="P15" s="13">
+      <c r="P15" s="5">
         <v>0.61446391232244502</v>
       </c>
-      <c r="Q15" s="13">
+      <c r="Q15" s="5">
         <v>0.61233660130718903</v>
       </c>
       <c r="R15" s="8">
@@ -3339,7 +3342,7 @@
       <c r="W15" s="5">
         <v>7.6136328224782501E-2</v>
       </c>
-      <c r="X15" s="10">
+      <c r="X15" s="9">
         <v>0.704105258299351</v>
       </c>
       <c r="Y15" s="4">
@@ -3430,9 +3433,9 @@
         <v>0.56168847554714296</v>
       </c>
     </row>
-    <row r="16" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>383</v>
@@ -3440,47 +3443,47 @@
       <c r="C16">
         <v>8</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="12">
         <f t="shared" si="0"/>
         <v>47.875</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="12">
         <v>1.2546583850931676</v>
       </c>
       <c r="F16" s="8">
         <v>0.62892561983470996</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="5">
         <v>0.62644628099173505</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="5">
         <v>0.615151515151515</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="5">
         <v>0.60606060606060597</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="5">
         <v>0.64187327823691398</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="5">
         <v>0.62809917355371903</v>
       </c>
       <c r="L16" s="8">
         <v>0.59864200746552798</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="5">
         <v>0.62425524007440703</v>
       </c>
-      <c r="N16" s="13">
+      <c r="N16" s="5">
         <v>0.60889786539577895</v>
       </c>
-      <c r="O16" s="13">
+      <c r="O16" s="5">
         <v>0.585314685314685</v>
       </c>
-      <c r="P16" s="13">
+      <c r="P16" s="5">
         <v>0.57315945856718298</v>
       </c>
-      <c r="Q16" s="13">
+      <c r="Q16" s="5">
         <v>0.58708576998050599</v>
       </c>
       <c r="R16" s="8">
@@ -3501,7 +3504,7 @@
       <c r="W16" s="5">
         <v>6.9578056657281395E-2</v>
       </c>
-      <c r="X16" s="10">
+      <c r="X16" s="9">
         <v>0.707037806418369</v>
       </c>
       <c r="Y16" s="4">
@@ -3592,9 +3595,9 @@
         <v>0.65018532703231502</v>
       </c>
     </row>
-    <row r="17" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>1192</v>
@@ -3602,47 +3605,47 @@
       <c r="C17">
         <v>21</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="12">
         <f t="shared" si="0"/>
         <v>56.761904761904759</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="12">
         <v>2.784126984126984</v>
       </c>
       <c r="F17" s="8">
         <v>0.70998322147651005</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="5">
         <v>0.71837248322147595</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="5">
         <v>0.718708053691275</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="5">
         <v>0.69127516778523401</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="5">
         <v>0.71560402684563695</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K17" s="5">
         <v>0.721476510067114</v>
       </c>
       <c r="L17" s="8">
         <v>0.641941315035644</v>
       </c>
-      <c r="M17" s="13">
+      <c r="M17" s="5">
         <v>0.63336532735990902</v>
       </c>
-      <c r="N17" s="13">
+      <c r="N17" s="5">
         <v>0.62494040501301396</v>
       </c>
-      <c r="O17" s="13">
+      <c r="O17" s="5">
         <v>0.620247863022372</v>
       </c>
-      <c r="P17" s="13">
+      <c r="P17" s="5">
         <v>0.61207537512925003</v>
       </c>
-      <c r="Q17" s="13">
+      <c r="Q17" s="5">
         <v>0.58498528999719801</v>
       </c>
       <c r="R17" s="8">
@@ -3663,7 +3666,7 @@
       <c r="W17" s="5">
         <v>7.0843311526731303E-2</v>
       </c>
-      <c r="X17" s="10">
+      <c r="X17" s="9">
         <v>0.65813003449274998</v>
       </c>
       <c r="Y17" s="4">
@@ -3754,9 +3757,9 @@
         <v>0.58642849957561705</v>
       </c>
     </row>
-    <row r="18" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>369</v>
@@ -3764,47 +3767,47 @@
       <c r="C18">
         <v>21</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="12">
         <f t="shared" si="0"/>
         <v>17.571428571428573</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="12">
         <v>2.7272727272727271</v>
       </c>
       <c r="F18" s="8">
         <v>0.78102981029810303</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="5">
         <v>0.77344173441734398</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="5">
         <v>0.77100271002709997</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="5">
         <v>0.76151761517615102</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="5">
         <v>0.75338753387533797</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="5">
         <v>0.76693766937669305</v>
       </c>
       <c r="L18" s="8">
         <v>0.72859924351213701</v>
       </c>
-      <c r="M18" s="13">
+      <c r="M18" s="5">
         <v>0.71364227324698304</v>
       </c>
-      <c r="N18" s="13">
+      <c r="N18" s="5">
         <v>0.72573787710194304</v>
       </c>
-      <c r="O18" s="13">
+      <c r="O18" s="5">
         <v>0.70539469427369705</v>
       </c>
-      <c r="P18" s="13">
+      <c r="P18" s="5">
         <v>0.71647956360186504</v>
       </c>
-      <c r="Q18" s="13">
+      <c r="Q18" s="5">
         <v>0.69066891281124099</v>
       </c>
       <c r="R18" s="8">
@@ -3825,7 +3828,7 @@
       <c r="W18" s="5">
         <v>6.6769514091534907E-2</v>
       </c>
-      <c r="X18" s="10">
+      <c r="X18" s="9">
         <v>0.614193475905919</v>
       </c>
       <c r="Y18" s="4">
@@ -3916,9 +3919,9 @@
         <v>0.49781879736863299</v>
       </c>
     </row>
-    <row r="19" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B19">
         <v>325</v>
@@ -3926,47 +3929,47 @@
       <c r="C19">
         <v>39</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="12">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="12">
         <v>6.7380952380952381</v>
       </c>
       <c r="F19" s="8">
         <v>0.85046153846153805</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="5">
         <v>0.85692307692307601</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="5">
         <v>0.84799999999999998</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="5">
         <v>0.86769230769230699</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="5">
         <v>0.86769230769230699</v>
       </c>
-      <c r="K19" s="13">
+      <c r="K19" s="5">
         <v>0.86153846153846103</v>
       </c>
       <c r="L19" s="8">
         <v>0.838244730902312</v>
       </c>
-      <c r="M19" s="13">
+      <c r="M19" s="5">
         <v>0.77026119186888298</v>
       </c>
-      <c r="N19" s="13">
+      <c r="N19" s="5">
         <v>0.79160154069442901</v>
       </c>
-      <c r="O19" s="13">
+      <c r="O19" s="5">
         <v>0.75366980042883003</v>
       </c>
-      <c r="P19" s="13">
+      <c r="P19" s="5">
         <v>0.68109846610588798</v>
       </c>
-      <c r="Q19" s="13">
+      <c r="Q19" s="5">
         <v>0.71619047619047604</v>
       </c>
       <c r="R19" s="8">
@@ -3987,7 +3990,7 @@
       <c r="W19" s="5">
         <v>5.4427812821589899E-2</v>
       </c>
-      <c r="X19" s="10">
+      <c r="X19" s="9">
         <v>0.31987399964820801</v>
       </c>
       <c r="Y19" s="4">
@@ -4078,9 +4081,9 @@
         <v>0.367040933841702</v>
       </c>
     </row>
-    <row r="20" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>341</v>
@@ -4088,47 +4091,47 @@
       <c r="C20">
         <v>6</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="12">
         <f t="shared" si="0"/>
         <v>56.833333333333336</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="12">
         <v>1.4014084507042253</v>
       </c>
       <c r="F20" s="8">
         <v>0.71524926686217005</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="5">
         <v>0.68621700879765302</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="5">
         <v>0.68445747800586498</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="5">
         <v>0.70087976539589403</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="5">
         <v>0.68621700879765302</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="5">
         <v>0.68328445747800504</v>
       </c>
       <c r="L20" s="8">
         <v>0.63731252657531701</v>
       </c>
-      <c r="M20" s="13">
+      <c r="M20" s="5">
         <v>0.63775261602364397</v>
       </c>
-      <c r="N20" s="13">
+      <c r="N20" s="5">
         <v>0.62528330991994796</v>
       </c>
-      <c r="O20" s="13">
+      <c r="O20" s="5">
         <v>0.62449749774386698</v>
       </c>
-      <c r="P20" s="13">
+      <c r="P20" s="5">
         <v>0.59745187315280701</v>
       </c>
-      <c r="Q20" s="13">
+      <c r="Q20" s="5">
         <v>0.63123907168971505</v>
       </c>
       <c r="R20" s="8">
@@ -4149,7 +4152,7 @@
       <c r="W20" s="5">
         <v>4.5773735472009303E-2</v>
       </c>
-      <c r="X20" s="10">
+      <c r="X20" s="9">
         <v>0.57520544432635301</v>
       </c>
       <c r="Y20" s="4">
@@ -4240,9 +4243,9 @@
         <v>0.59257525169830205</v>
       </c>
     </row>
-    <row r="21" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>104</v>
@@ -4250,47 +4253,47 @@
       <c r="C21">
         <v>8</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="12">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="12">
         <v>1.1224489795918366</v>
       </c>
       <c r="F21" s="8">
         <v>0.6875</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="5">
         <v>0.62115384615384595</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="5">
         <v>0.68269230769230704</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="5">
         <v>0.61538461538461497</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="5">
         <v>0.56730769230769196</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="5">
         <v>0.68269230769230704</v>
       </c>
       <c r="L21" s="8">
         <v>0.61027649273803097</v>
       </c>
-      <c r="M21" s="13">
+      <c r="M21" s="5">
         <v>0.64233824708082499</v>
       </c>
-      <c r="N21" s="13">
+      <c r="N21" s="5">
         <v>0.55084933845497197</v>
       </c>
-      <c r="O21" s="13">
+      <c r="O21" s="5">
         <v>0.65839843749999905</v>
       </c>
-      <c r="P21" s="13">
+      <c r="P21" s="5">
         <v>0.61600753295668498</v>
       </c>
-      <c r="Q21" s="13">
+      <c r="Q21" s="5">
         <v>0.483781476739223</v>
       </c>
       <c r="R21" s="8">
@@ -4311,7 +4314,7 @@
       <c r="W21" s="5">
         <v>0.13297972828149701</v>
       </c>
-      <c r="X21" s="10">
+      <c r="X21" s="9">
         <v>0.67598859327872396</v>
       </c>
       <c r="Y21" s="4">
@@ -4402,9 +4405,9 @@
         <v>0.64016838191298198</v>
       </c>
     </row>
-    <row r="22" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B22">
         <v>1343</v>
@@ -4412,47 +4415,47 @@
       <c r="C22">
         <v>37</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="12">
         <f t="shared" si="0"/>
         <v>36.297297297297298</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="12">
         <v>6.5875706214689265</v>
       </c>
       <c r="F22" s="8">
         <v>0.89553239017125796</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="5">
         <v>0.89113924050632898</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="5">
         <v>0.88830975428145897</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="5">
         <v>0.89650037230081903</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="5">
         <v>0.88682055100521195</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="5">
         <v>0.88756515264333502</v>
       </c>
       <c r="L22" s="8">
         <v>0.90624361994730196</v>
       </c>
-      <c r="M22" s="13">
+      <c r="M22" s="5">
         <v>0.88903994784084495</v>
       </c>
-      <c r="N22" s="13">
+      <c r="N22" s="5">
         <v>0.89012059234423002</v>
       </c>
-      <c r="O22" s="13">
+      <c r="O22" s="5">
         <v>0.91443390138387604</v>
       </c>
-      <c r="P22" s="13">
+      <c r="P22" s="5">
         <v>0.86971364178708699</v>
       </c>
-      <c r="Q22" s="13">
+      <c r="Q22" s="5">
         <v>0.90424574425530002</v>
       </c>
       <c r="R22" s="8">
@@ -4473,7 +4476,7 @@
       <c r="W22" s="5">
         <v>2.29359970647184E-2</v>
       </c>
-      <c r="X22" s="10">
+      <c r="X22" s="9">
         <v>0.21745900758502401</v>
       </c>
       <c r="Y22" s="4">
@@ -4564,9 +4567,9 @@
         <v>0.224577695187995</v>
       </c>
     </row>
-    <row r="23" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B23">
         <v>208</v>
@@ -4574,47 +4577,47 @@
       <c r="C23">
         <v>60</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="12">
         <f t="shared" si="0"/>
         <v>3.4666666666666668</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="12">
         <v>1.1443298969072164</v>
       </c>
       <c r="F23" s="8">
         <v>0.72067307692307603</v>
       </c>
-      <c r="G23" s="13">
+      <c r="G23" s="5">
         <v>0.6875</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="5">
         <v>0.65913461538461504</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="5">
         <v>0.73557692307692302</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="5">
         <v>0.68269230769230704</v>
       </c>
-      <c r="K23" s="13">
+      <c r="K23" s="5">
         <v>0.66826923076922995</v>
       </c>
       <c r="L23" s="8">
         <v>0.72968783549331195</v>
       </c>
-      <c r="M23" s="13">
+      <c r="M23" s="5">
         <v>0.68482947821409301</v>
       </c>
-      <c r="N23" s="13">
+      <c r="N23" s="5">
         <v>0.69408994906582899</v>
       </c>
-      <c r="O23" s="13">
+      <c r="O23" s="5">
         <v>0.72929292929292899</v>
       </c>
-      <c r="P23" s="13">
+      <c r="P23" s="5">
         <v>0.69184805804524097</v>
       </c>
-      <c r="Q23" s="13">
+      <c r="Q23" s="5">
         <v>0.72901678657074298</v>
       </c>
       <c r="R23" s="8">
@@ -4635,7 +4638,7 @@
       <c r="W23" s="5">
         <v>0.14568072745504801</v>
       </c>
-      <c r="X23" s="10">
+      <c r="X23" s="9">
         <v>0.53241085719136205</v>
       </c>
       <c r="Y23" s="4">
@@ -4726,9 +4729,9 @@
         <v>0.57904062345762597</v>
       </c>
     </row>
-    <row r="24" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>218</v>
@@ -4736,47 +4739,47 @@
       <c r="C24">
         <v>22</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="12">
         <f t="shared" si="0"/>
         <v>9.9090909090909083</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="12">
         <v>8.0833333333333339</v>
       </c>
       <c r="F24" s="8">
         <v>0.87706422018348595</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="5">
         <v>0.88990825688073305</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="5">
         <v>0.87247706422018301</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="5">
         <v>0.85779816513761398</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="5">
         <v>0.88532110091743099</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="5">
         <v>0.86697247706421998</v>
       </c>
       <c r="L24" s="8">
         <v>0.66305794510710003</v>
       </c>
-      <c r="M24" s="13">
+      <c r="M24" s="5">
         <v>0.50866408934707896</v>
       </c>
-      <c r="N24" s="13">
+      <c r="N24" s="5">
         <v>0.64260452836468995</v>
       </c>
-      <c r="O24" s="13">
+      <c r="O24" s="5">
         <v>0.75211316198033396</v>
       </c>
-      <c r="P24" s="13">
+      <c r="P24" s="5">
         <v>0.61119170984455895</v>
       </c>
-      <c r="Q24" s="13">
+      <c r="Q24" s="5">
         <v>0.71100164203612404</v>
       </c>
       <c r="R24" s="8">
@@ -4797,7 +4800,7 @@
       <c r="W24" s="5">
         <v>6.0718322018964502E-2</v>
       </c>
-      <c r="X24" s="10">
+      <c r="X24" s="9">
         <v>0.39169713149938601</v>
       </c>
       <c r="Y24" s="4">
@@ -4888,9 +4891,9 @@
         <v>0.334506589419232</v>
       </c>
     </row>
-    <row r="25" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B25">
         <v>267</v>
@@ -4898,47 +4901,47 @@
       <c r="C25">
         <v>44</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="12">
         <f t="shared" si="0"/>
         <v>6.0681818181818183</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="12">
         <v>3.8545454545454545</v>
       </c>
       <c r="F25" s="8">
         <v>0.80936329588014899</v>
       </c>
-      <c r="G25" s="13">
+      <c r="G25" s="5">
         <v>0.78951310861423196</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="5">
         <v>0.79101123595505596</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="5">
         <v>0.80898876404494302</v>
       </c>
-      <c r="J25" s="13">
+      <c r="J25" s="5">
         <v>0.77902621722846399</v>
       </c>
-      <c r="K25" s="13">
+      <c r="K25" s="5">
         <v>0.78277153558052404</v>
       </c>
       <c r="L25" s="8">
         <v>0.81928843973675103</v>
       </c>
-      <c r="M25" s="13">
+      <c r="M25" s="5">
         <v>0.80836138553687997</v>
       </c>
-      <c r="N25" s="13">
+      <c r="N25" s="5">
         <v>0.78237049595416497</v>
       </c>
-      <c r="O25" s="13">
+      <c r="O25" s="5">
         <v>0.73157225853304297</v>
       </c>
-      <c r="P25" s="13">
+      <c r="P25" s="5">
         <v>0.73142112125162895</v>
       </c>
-      <c r="Q25" s="13">
+      <c r="Q25" s="5">
         <v>0.78303910245833996</v>
       </c>
       <c r="R25" s="8">
@@ -4959,7 +4962,7 @@
       <c r="W25" s="5">
         <v>5.6206491751394E-2</v>
       </c>
-      <c r="X25" s="10">
+      <c r="X25" s="9">
         <v>0.38417114056852902</v>
       </c>
       <c r="Y25" s="4">
@@ -5050,9 +5053,9 @@
         <v>0.43157610667465801</v>
       </c>
     </row>
-    <row r="26" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B26">
         <v>502</v>
@@ -5060,47 +5063,47 @@
       <c r="C26">
         <v>4</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="12">
         <f t="shared" si="0"/>
         <v>125.5</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="12">
         <v>2.83206106870229</v>
       </c>
       <c r="F26" s="8">
         <v>0.65717131474103496</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="5">
         <v>0.70199203187250903</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="5">
         <v>0.69442231075697203</v>
       </c>
-      <c r="I26" s="13">
+      <c r="I26" s="5">
         <v>0.65737051792828605</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="5">
         <v>0.69920318725099595</v>
       </c>
-      <c r="K26" s="13">
+      <c r="K26" s="5">
         <v>0.67729083665338596</v>
       </c>
       <c r="L26" s="8">
         <v>0.58920677281637102</v>
       </c>
-      <c r="M26" s="13">
+      <c r="M26" s="5">
         <v>0.60208190437458597</v>
       </c>
-      <c r="N26" s="13">
+      <c r="N26" s="5">
         <v>0.58774799327688798</v>
       </c>
-      <c r="O26" s="13">
+      <c r="O26" s="5">
         <v>0.63152748414376303</v>
       </c>
-      <c r="P26" s="13">
+      <c r="P26" s="5">
         <v>0.62640327540989804</v>
       </c>
-      <c r="Q26" s="13">
+      <c r="Q26" s="5">
         <v>0.67226761074800201</v>
       </c>
       <c r="R26" s="8">
@@ -5121,7 +5124,7 @@
       <c r="W26" s="5">
         <v>9.4806452931101501E-2</v>
       </c>
-      <c r="X26" s="10">
+      <c r="X26" s="9">
         <v>1.08062351260431</v>
       </c>
       <c r="Y26" s="4">
@@ -5212,9 +5215,9 @@
         <v>0.55489815282370603</v>
       </c>
     </row>
-    <row r="27" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B27">
         <v>958</v>
@@ -5222,47 +5225,47 @@
       <c r="C27">
         <v>27</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="12">
         <f t="shared" si="0"/>
         <v>35.481481481481481</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="12">
         <v>1.8855421686746987</v>
       </c>
       <c r="F27" s="8">
         <v>0.91931106471816204</v>
       </c>
-      <c r="G27" s="13">
+      <c r="G27" s="5">
         <v>0.89509394572025003</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="5">
         <v>0.89144050104384098</v>
       </c>
-      <c r="I27" s="13">
+      <c r="I27" s="5">
         <v>0.87369519832985298</v>
       </c>
-      <c r="J27" s="13">
+      <c r="J27" s="5">
         <v>0.88935281837160696</v>
       </c>
-      <c r="K27" s="13">
+      <c r="K27" s="5">
         <v>0.88308977035490599</v>
       </c>
       <c r="L27" s="8">
         <v>0.87640116624859199</v>
       </c>
-      <c r="M27" s="13">
+      <c r="M27" s="5">
         <v>0.82977810655178896</v>
       </c>
-      <c r="N27" s="13">
+      <c r="N27" s="5">
         <v>0.82508202350927695</v>
       </c>
-      <c r="O27" s="13">
+      <c r="O27" s="5">
         <v>0.85969173652458097</v>
       </c>
-      <c r="P27" s="13">
+      <c r="P27" s="5">
         <v>0.74400411905394603</v>
       </c>
-      <c r="Q27" s="13">
+      <c r="Q27" s="5">
         <v>0.81752891759540602</v>
       </c>
       <c r="R27" s="8">
@@ -5283,7 +5286,7 @@
       <c r="W27" s="5">
         <v>6.7335686241014006E-2</v>
       </c>
-      <c r="X27" s="10">
+      <c r="X27" s="9">
         <v>0.32090881019237499</v>
       </c>
       <c r="Y27" s="4">
@@ -5374,9 +5377,9 @@
         <v>0.29044356787176401</v>
       </c>
     </row>
-    <row r="28" spans="1:64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B28">
         <v>517</v>
@@ -5384,47 +5387,47 @@
       <c r="C28">
         <v>16</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="12">
         <f t="shared" si="0"/>
         <v>32.3125</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="12">
         <v>2.9791666666666665</v>
       </c>
       <c r="F28" s="8">
         <v>0.81818181818181801</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="5">
         <v>0.79903288201160505</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="5">
         <v>0.81179883945841302</v>
       </c>
-      <c r="I28" s="13">
+      <c r="I28" s="5">
         <v>0.800773694390715</v>
       </c>
-      <c r="J28" s="13">
+      <c r="J28" s="5">
         <v>0.77562862669245602</v>
       </c>
-      <c r="K28" s="13">
+      <c r="K28" s="5">
         <v>0.779497098646034</v>
       </c>
       <c r="L28" s="8">
         <v>0.72341921935516296</v>
       </c>
-      <c r="M28" s="13">
+      <c r="M28" s="5">
         <v>0.64729495453167596</v>
       </c>
-      <c r="N28" s="13">
+      <c r="N28" s="5">
         <v>0.65270891629390204</v>
       </c>
-      <c r="O28" s="13">
+      <c r="O28" s="5">
         <v>0.73791097978518805</v>
       </c>
-      <c r="P28" s="13">
+      <c r="P28" s="5">
         <v>0.60611402528162295</v>
       </c>
-      <c r="Q28" s="13">
+      <c r="Q28" s="5">
         <v>0.66450089242958499</v>
       </c>
       <c r="R28" s="8">
@@ -5445,7 +5448,7 @@
       <c r="W28" s="5">
         <v>0.110493817170307</v>
       </c>
-      <c r="X28" s="10">
+      <c r="X28" s="9">
         <v>0.46289376552468198</v>
       </c>
       <c r="Y28" s="4">
@@ -5536,165 +5539,165 @@
         <v>0.464803342161277</v>
       </c>
     </row>
-    <row r="29" spans="1:64" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="19">
+    <row r="29" spans="1:64" s="3" customFormat="1">
+      <c r="A29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="3">
         <v>463</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="3">
         <v>9</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="14">
         <f t="shared" si="0"/>
         <v>51.444444444444443</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="14">
         <v>1.1688888888888889</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="15">
         <v>0.95075593952483795</v>
       </c>
-      <c r="G29" s="22">
+      <c r="G29" s="16">
         <v>0.94146868250539895</v>
       </c>
-      <c r="H29" s="22">
+      <c r="H29" s="16">
         <v>0.94578833693304498</v>
       </c>
-      <c r="I29" s="22">
+      <c r="I29" s="16">
         <v>0.92872570194384396</v>
       </c>
-      <c r="J29" s="22">
+      <c r="J29" s="16">
         <v>0.93088552915766698</v>
       </c>
-      <c r="K29" s="22">
+      <c r="K29" s="16">
         <v>0.93304535637149</v>
       </c>
-      <c r="L29" s="21">
+      <c r="L29" s="15">
         <v>0.84395649505408199</v>
       </c>
-      <c r="M29" s="22">
+      <c r="M29" s="16">
         <v>0.86951838203860299</v>
       </c>
-      <c r="N29" s="22">
+      <c r="N29" s="16">
         <v>0.85072953220231595</v>
       </c>
-      <c r="O29" s="22">
+      <c r="O29" s="16">
         <v>0.89027484143763203</v>
       </c>
-      <c r="P29" s="22">
+      <c r="P29" s="16">
         <v>0.71925754060324798</v>
       </c>
-      <c r="Q29" s="22">
+      <c r="Q29" s="16">
         <v>0.83318399044205405</v>
       </c>
-      <c r="R29" s="21">
+      <c r="R29" s="15">
         <v>2.6833695775103E-2</v>
       </c>
-      <c r="S29" s="22">
+      <c r="S29" s="16">
         <v>2.9332174787189101E-2</v>
       </c>
-      <c r="T29" s="22">
+      <c r="T29" s="16">
         <v>4.7181556631306E-2</v>
       </c>
-      <c r="U29" s="22">
+      <c r="U29" s="16">
         <v>4.8349109367536801E-2</v>
       </c>
-      <c r="V29" s="22">
+      <c r="V29" s="16">
         <v>2.2722029434939402E-2</v>
       </c>
-      <c r="W29" s="22">
+      <c r="W29" s="16">
         <v>4.77010507647503E-2</v>
       </c>
-      <c r="X29" s="23">
+      <c r="X29" s="17">
         <v>0.16756513755540101</v>
       </c>
-      <c r="Y29" s="24">
+      <c r="Y29" s="18">
         <v>0.16683197405389699</v>
       </c>
-      <c r="Z29" s="24">
+      <c r="Z29" s="18">
         <v>0.18107089839562801</v>
       </c>
-      <c r="AA29" s="24">
+      <c r="AA29" s="18">
         <v>0.22088777442413601</v>
       </c>
-      <c r="AB29" s="24">
+      <c r="AB29" s="18">
         <v>0.22604899528083</v>
       </c>
-      <c r="AC29" s="24">
+      <c r="AC29" s="18">
         <v>0.211658158424154</v>
       </c>
-      <c r="AD29" s="21">
+      <c r="AD29" s="15">
         <v>5.7269503873160502E-2</v>
       </c>
-      <c r="AE29" s="22">
+      <c r="AE29" s="16">
         <v>3.9667348774502002E-2</v>
       </c>
-      <c r="AF29" s="22">
+      <c r="AF29" s="16">
         <v>6.6078385013199195E-2</v>
       </c>
-      <c r="AG29" s="22">
+      <c r="AG29" s="16">
         <v>3.62268026870399E-2</v>
       </c>
-      <c r="AH29" s="22">
+      <c r="AH29" s="16">
         <v>4.6853690755524403E-2</v>
       </c>
-      <c r="AI29" s="22">
+      <c r="AI29" s="16">
         <v>5.7761693813634399E-2</v>
       </c>
-      <c r="AJ29" s="21">
+      <c r="AJ29" s="15">
         <v>4.3824555726542203E-2</v>
       </c>
-      <c r="AK29" s="22">
+      <c r="AK29" s="16">
         <v>3.6710040081755699E-2</v>
       </c>
-      <c r="AL29" s="22">
+      <c r="AL29" s="16">
         <v>5.0985364429323499E-2</v>
       </c>
-      <c r="AM29" s="22">
+      <c r="AM29" s="16">
         <v>3.2948781435330698E-2</v>
       </c>
-      <c r="AN29" s="22">
+      <c r="AN29" s="16">
         <v>3.5829348899367203E-2</v>
       </c>
-      <c r="AO29" s="22">
+      <c r="AO29" s="16">
         <v>4.28608690941326E-2</v>
       </c>
-      <c r="AP29" s="21">
+      <c r="AP29" s="15">
         <v>0.31074071942230802</v>
       </c>
-      <c r="AQ29" s="22">
+      <c r="AQ29" s="16">
         <v>0.62497618435151703</v>
       </c>
-      <c r="AR29" s="22">
+      <c r="AR29" s="16">
         <v>0.337698400675217</v>
       </c>
-      <c r="AS29" s="22">
+      <c r="AS29" s="16">
         <v>0.86579897905828296</v>
       </c>
-      <c r="AT29" s="22">
+      <c r="AT29" s="16">
         <v>0.80622459604049102</v>
       </c>
-      <c r="AU29" s="22">
+      <c r="AU29" s="16">
         <v>0.289064345478176</v>
       </c>
-      <c r="AV29" s="21">
+      <c r="AV29" s="15">
         <v>0.29592589502844602</v>
       </c>
-      <c r="AW29" s="22">
+      <c r="AW29" s="16">
         <v>0.41466127469719199</v>
       </c>
-      <c r="AX29" s="22">
+      <c r="AX29" s="16">
         <v>0.18232322592873301</v>
       </c>
-      <c r="AY29" s="22">
+      <c r="AY29" s="16">
         <v>0.57142084249616298</v>
       </c>
-      <c r="AZ29" s="22">
+      <c r="AZ29" s="16">
         <v>0.513856136730232</v>
       </c>
-      <c r="BA29" s="22">
+      <c r="BA29" s="16">
         <v>0.20404483995054101</v>
       </c>
       <c r="BB29"/>
@@ -5709,276 +5712,279 @@
       <c r="BK29"/>
       <c r="BL29"/>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="16">
+    <row r="30" spans="1:64" ht="15">
+      <c r="A30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="30">
         <f>AVERAGE(B5:B29)</f>
         <v>476.04</v>
       </c>
-      <c r="C30" s="16">
+      <c r="C30" s="30">
         <f t="shared" ref="C30:W30" si="1">AVERAGE(C5:C29)</f>
         <v>23.04</v>
       </c>
-      <c r="D30" s="16">
+      <c r="D30" s="30">
         <f t="shared" si="1"/>
         <v>34.040133151689353</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="30">
         <f t="shared" si="1"/>
         <v>2.6063570204851692</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="31">
         <f t="shared" si="1"/>
         <v>0.79090580946276967</v>
       </c>
-      <c r="G30" s="17">
+      <c r="G30" s="32">
         <f t="shared" si="1"/>
         <v>0.7866301577695376</v>
       </c>
-      <c r="H30" s="17">
+      <c r="H30" s="33">
         <f t="shared" si="1"/>
         <v>0.78364932685072564</v>
       </c>
-      <c r="I30" s="17">
+      <c r="I30" s="32">
         <f t="shared" si="1"/>
         <v>0.7664275113878618</v>
       </c>
-      <c r="J30" s="17">
+      <c r="J30" s="32">
         <f t="shared" si="1"/>
         <v>0.77714859630764044</v>
       </c>
-      <c r="K30" s="17">
+      <c r="K30" s="32">
         <f t="shared" si="1"/>
         <v>0.77543480722288971</v>
       </c>
-      <c r="L30" s="18">
+      <c r="L30" s="31">
         <f t="shared" si="1"/>
         <v>0.73567126554018913</v>
       </c>
-      <c r="M30" s="17">
+      <c r="M30" s="33">
         <f t="shared" si="1"/>
         <v>0.71236978627668956</v>
       </c>
-      <c r="N30" s="17">
+      <c r="N30" s="33">
         <f t="shared" si="1"/>
         <v>0.71439592343109171</v>
       </c>
-      <c r="O30" s="17">
+      <c r="O30" s="32">
         <f t="shared" si="1"/>
         <v>0.73230080619116411</v>
       </c>
-      <c r="P30" s="17">
+      <c r="P30" s="33">
         <f t="shared" si="1"/>
         <v>0.65410715016663001</v>
       </c>
-      <c r="Q30" s="17">
+      <c r="Q30" s="33">
         <f t="shared" si="1"/>
         <v>0.69590458849899961</v>
       </c>
-      <c r="R30" s="18">
+      <c r="R30" s="31">
         <f t="shared" si="1"/>
         <v>6.8729853777899239E-2</v>
       </c>
-      <c r="S30" s="17">
+      <c r="S30" s="32">
         <f t="shared" si="1"/>
         <v>5.402246748524614E-2</v>
       </c>
-      <c r="T30" s="17">
+      <c r="T30" s="32">
         <f t="shared" si="1"/>
         <v>5.3158466043211831E-2</v>
       </c>
-      <c r="U30" s="17">
+      <c r="U30" s="32">
         <f t="shared" si="1"/>
         <v>0.14984646432503299</v>
       </c>
-      <c r="V30" s="17">
+      <c r="V30" s="13">
         <f t="shared" si="1"/>
         <v>6.274847973753879E-2</v>
       </c>
-      <c r="W30" s="17">
+      <c r="W30" s="13">
         <f t="shared" si="1"/>
         <v>6.9209901201573679E-2</v>
       </c>
-      <c r="X30" s="18">
+      <c r="X30" s="31">
         <v>0.48268667348845107</v>
       </c>
-      <c r="Y30" s="17">
+      <c r="Y30" s="32">
         <v>0.44570893608516016</v>
       </c>
-      <c r="Z30" s="17">
+      <c r="Z30" s="32">
         <v>0.44967823831084541</v>
       </c>
-      <c r="AA30" s="17">
+      <c r="AA30" s="32">
         <v>0.62845776215774873</v>
       </c>
-      <c r="AB30" s="17">
+      <c r="AB30" s="13">
         <v>0.48158381138320638</v>
       </c>
-      <c r="AC30" s="17">
+      <c r="AC30" s="13">
         <v>0.46864656136949495</v>
       </c>
-      <c r="AD30" s="18">
+      <c r="AD30" s="31">
         <v>7.2662062306540903E-2</v>
       </c>
-      <c r="AE30" s="17">
+      <c r="AE30" s="32">
         <v>6.5316928737798569E-2</v>
       </c>
-      <c r="AF30" s="17">
+      <c r="AF30" s="32">
         <v>7.4785873014055856E-2</v>
       </c>
-      <c r="AG30" s="17">
+      <c r="AG30" s="32">
         <v>0.11187667812331302</v>
       </c>
-      <c r="AH30" s="17">
+      <c r="AH30" s="13">
         <v>7.5782263475973555E-2</v>
       </c>
-      <c r="AI30" s="17">
+      <c r="AI30" s="13">
         <v>7.488959791300133E-2</v>
       </c>
-      <c r="AJ30" s="18">
+      <c r="AJ30" s="31">
         <v>6.5995958009024913E-2</v>
       </c>
-      <c r="AK30" s="17">
+      <c r="AK30" s="32">
         <v>5.8651775484677815E-2</v>
       </c>
-      <c r="AL30" s="17">
+      <c r="AL30" s="32">
         <v>6.1871510031437732E-2</v>
       </c>
-      <c r="AM30" s="17">
+      <c r="AM30" s="32">
         <v>0.10703986319980277</v>
       </c>
-      <c r="AN30" s="17">
+      <c r="AN30" s="13">
         <v>5.9380759915040986E-2</v>
       </c>
-      <c r="AO30" s="17">
+      <c r="AO30" s="13">
         <v>6.6492394495848248E-2</v>
       </c>
-      <c r="AP30" s="17">
+      <c r="AP30" s="32">
         <v>0.64375655849409197</v>
       </c>
-      <c r="AQ30" s="17">
+      <c r="AQ30" s="32">
         <v>0.75399060665292139</v>
       </c>
-      <c r="AR30" s="17">
+      <c r="AR30" s="32">
         <v>0.67442121552834167</v>
       </c>
-      <c r="AS30" s="17">
+      <c r="AS30" s="32">
         <v>1.6860848051491282</v>
       </c>
-      <c r="AT30" s="17">
+      <c r="AT30" s="13">
         <v>0.84381454397615141</v>
       </c>
-      <c r="AU30" s="17">
+      <c r="AU30" s="13">
         <v>0.73860566478557654</v>
       </c>
-      <c r="AV30" s="18">
+      <c r="AV30" s="31">
         <v>0.47253896257439565</v>
       </c>
-      <c r="AW30" s="17">
+      <c r="AW30" s="32">
         <v>0.47129969994829424</v>
       </c>
-      <c r="AX30" s="17">
+      <c r="AX30" s="32">
         <v>0.45769529682487542</v>
       </c>
-      <c r="AY30" s="17">
+      <c r="AY30" s="32">
         <v>0.97657232348830381</v>
       </c>
-      <c r="AZ30" s="17">
+      <c r="AZ30" s="13">
         <v>0.48534828099321969</v>
       </c>
-      <c r="BA30" s="17">
+      <c r="BA30" s="13">
         <v>0.46509642244084404</v>
       </c>
-      <c r="BB30"/>
-      <c r="BC30"/>
-      <c r="BD30"/>
-      <c r="BE30"/>
-      <c r="BF30"/>
-      <c r="BG30"/>
-      <c r="BH30"/>
-      <c r="BI30"/>
-      <c r="BJ30"/>
-      <c r="BK30"/>
-      <c r="BL30"/>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="AP31"/>
-      <c r="AQ31"/>
-      <c r="AR31"/>
-      <c r="AS31"/>
-      <c r="AT31"/>
-      <c r="AU31"/>
-      <c r="AV31"/>
-      <c r="AW31"/>
-      <c r="AX31"/>
-      <c r="AY31"/>
-      <c r="AZ31"/>
-      <c r="BA31"/>
-      <c r="BB31"/>
-      <c r="BC31"/>
-      <c r="BD31"/>
-      <c r="BE31"/>
-      <c r="BF31"/>
-      <c r="BG31"/>
-      <c r="BH31"/>
-      <c r="BI31"/>
-      <c r="BJ31"/>
-      <c r="BK31"/>
-      <c r="BL31"/>
+    <row r="31" spans="1:64">
+      <c r="H31" t="s">
+        <v>47</v>
+      </c>
+      <c r="M31" t="s">
+        <v>47</v>
+      </c>
+      <c r="N31" t="s">
+        <v>47</v>
+      </c>
+      <c r="P31" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>47</v>
+      </c>
+      <c r="V31" t="s">
+        <v>48</v>
+      </c>
+      <c r="W31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AU31" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ31" t="s">
+        <v>48</v>
+      </c>
+      <c r="BA31" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="32" spans="1:64" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
-      <c r="W32" s="9"/>
-      <c r="X32" s="9"/>
-    </row>
-    <row r="33" spans="1:24" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
-      <c r="W33" s="9"/>
-      <c r="X33" s="9"/>
-    </row>
-    <row r="34" spans="1:24" customFormat="1" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="U34" s="9"/>
-      <c r="V34" s="9"/>
-      <c r="W34" s="9"/>
-      <c r="X34" s="9"/>
-    </row>
-    <row r="35" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:24" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:64" ht="10.15" customHeight="1"/>
+    <row r="33" ht="10.15" customHeight="1"/>
+    <row r="34" ht="10.15" customHeight="1"/>
+    <row r="35" ht="10.15" customHeight="1"/>
+    <row r="36" ht="10.15" customHeight="1"/>
+    <row r="37" ht="10.15" customHeight="1"/>
+    <row r="38" ht="10.15" customHeight="1"/>
+    <row r="39" ht="10.15" customHeight="1"/>
+    <row r="40" ht="10.15" customHeight="1"/>
+    <row r="41" ht="10.15" customHeight="1"/>
+    <row r="42" ht="10.15" customHeight="1"/>
+    <row r="43" ht="10.15" customHeight="1"/>
+    <row r="44" ht="10.15" customHeight="1"/>
+    <row r="45" ht="10.15" customHeight="1"/>
+    <row r="46" ht="10.15" customHeight="1"/>
+    <row r="47" ht="10.15" customHeight="1"/>
+    <row r="48" ht="10.15" customHeight="1"/>
+    <row r="49" ht="10.15" customHeight="1"/>
+    <row r="50" ht="10.15" customHeight="1"/>
+    <row r="51" ht="10.15" customHeight="1"/>
+    <row r="52" ht="10.15" customHeight="1"/>
+    <row r="53" ht="10.15" customHeight="1"/>
+    <row r="54" ht="10.15" customHeight="1"/>
+    <row r="55" ht="10.15" customHeight="1"/>
+    <row r="56" ht="10.15" customHeight="1"/>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="AM3:AO3"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="AD1:AO1"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="L2:Q2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="O3:Q3"/>
     <mergeCell ref="X3:Z3"/>
     <mergeCell ref="AA3:AC3"/>
     <mergeCell ref="AD2:AI2"/>
@@ -5986,12 +5992,10 @@
     <mergeCell ref="AD3:AF3"/>
     <mergeCell ref="AG3:AI3"/>
     <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AM3:AO3"/>
-    <mergeCell ref="L2:Q2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AS3:AU3"/>
+    <mergeCell ref="AV3:AX3"/>
+    <mergeCell ref="AY3:BA3"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:Q1"/>
     <mergeCell ref="AP1:BA1"/>
@@ -6004,14 +6008,6 @@
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="R2:W2"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="AD1:AO1"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AS3:AU3"/>
-    <mergeCell ref="AV3:AX3"/>
-    <mergeCell ref="AY3:BA3"/>
   </mergeCells>
   <conditionalFormatting sqref="R5:T29">
     <cfRule type="colorScale" priority="70">
@@ -6474,39 +6470,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{357B6B06-B783-42EF-BCD1-E6138D497C98}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8b3620b1-e6be-49c9-b068-45226c8b10d8"/>
-    <ds:schemaRef ds:uri="37d4d6e9-8180-42d6-bff6-05dffb4cfa48"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{357B6B06-B783-42EF-BCD1-E6138D497C98}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7B693C6-2878-481A-A484-920847E6C5EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7B693C6-2878-481A-A484-920847E6C5EC}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E6BD3BF-5D5D-4FEB-8EB4-3B7C274804EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8b3620b1-e6be-49c9-b068-45226c8b10d8"/>
-    <ds:schemaRef ds:uri="37d4d6e9-8180-42d6-bff6-05dffb4cfa48"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E6BD3BF-5D5D-4FEB-8EB4-3B7C274804EF}"/>
 </file>
</xml_diff>